<commit_message>
Entrega Final - Laboratorio 4
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 maquina 2.xlsx
+++ b/Docs/Tablas Lab 4 maquina 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maicol -PC\Documents\Lab 4\LabSorts-S04-G10\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59F2632-EFC7-484E-87FA-436D62CF0BCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,7 +459,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +526,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,17 +613,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -635,63 +635,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>5406.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>29109.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>139640.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>662125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,17 +745,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -803,63 +767,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>38968.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>140953.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>661968.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,17 +876,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -970,63 +898,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
+              <c:f>'Datos Lab4'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5531.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>98921.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>140109.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>662437.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1126,7 +1018,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1164,7 +1056,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1248,7 +1140,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1286,7 +1178,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1328,7 +1220,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1365,7 +1257,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1374,7 +1266,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1441,7 +1333,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1456,7 +1348,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$B$14</c:f>
+              <c:f>'Datos Lab4'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1528,17 +1420,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$9:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1550,63 +1442,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4'!$B$9:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>5359.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>29578.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>140343.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>662022.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,7 +1479,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$C$14</c:f>
+              <c:f>'Datos Lab4'!$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1696,85 +1552,49 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5359.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>29765.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>142187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>663198.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5359.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>29765.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>142187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>663198.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1791,7 +1611,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$D$14</c:f>
+              <c:f>'Datos Lab4'!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1863,17 +1683,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$9:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1885,63 +1705,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4'!$D$9:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>5531.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>28984.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>141359.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>660112.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2041,7 +1825,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2079,7 +1863,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -2163,7 +1947,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2201,7 +1985,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2243,7 +2027,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2280,7 +2064,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2289,7 +2073,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2356,7 +2140,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2444,17 +2228,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2466,63 +2250,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
+              <c:f>'Datos Lab4'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>5406.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>29109.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>139640.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>662125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2539,7 +2287,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$B$14</c:f>
+              <c:f>'Datos Lab4'!$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2612,17 +2360,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$9:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2634,63 +2382,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
+              <c:f>'Datos Lab4'!$B$9:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>5359.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>29578.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70</c:v>
+                  <c:v>140343.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>140</c:v>
+                  <c:v>662022.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,7 +2502,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2828,7 +2540,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2907,7 +2619,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2945,7 +2657,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2987,7 +2699,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3024,7 +2736,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3033,7 +2745,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3095,7 +2807,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,17 +2895,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3205,63 +2917,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
+              <c:f>'Datos Lab4'!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>38968.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>140953.125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>661968.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3278,7 +2954,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$C$14</c:f>
+              <c:f>'Datos Lab4'!$C$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3351,17 +3027,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$9:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3373,63 +3049,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:f>'Datos Lab4'!$C$9:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5359.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>29765.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>142187.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>178</c:v>
+                  <c:v>663198.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3529,7 +3169,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3567,7 +3207,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3646,7 +3286,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3684,7 +3324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3726,7 +3366,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3763,7 +3403,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3772,7 +3412,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3834,7 +3474,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3922,17 +3562,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
+              <c:f>'Datos Lab4'!$A$2:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3944,63 +3584,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
+              <c:f>'Datos Lab4'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5531.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>98921.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>140109.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>662437.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4017,7 +3621,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos Lab4'!$D$14</c:f>
+              <c:f>'Datos Lab4'!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4090,17 +3694,17 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-419"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
+              <c:f>'Datos Lab4'!$A$9:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -4112,63 +3716,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>256000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>512000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
+              <c:f>'Datos Lab4'!$D$9:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>5531.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78</c:v>
+                  <c:v>28984.375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>141359.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>148</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>158</c:v>
+                  <c:v>660112.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4268,7 +3836,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4306,7 +3874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -4385,7 +3953,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-419"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4423,7 +3991,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-419"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4465,7 +4033,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-419"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4502,7 +4070,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-419"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -7286,7 +6854,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7297,7 +6865,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7308,7 +6876,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7319,7 +6887,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7330,7 +6898,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="74" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7341,7 +6909,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9319054" cy="6088277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7374,7 +6942,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9319054" cy="6088277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7407,7 +6975,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9319054" cy="6088277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7440,7 +7008,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9319054" cy="6088277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7473,7 +7041,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9319054" cy="6088277"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7503,8 +7071,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:D5" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
@@ -7516,8 +7084,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A8:D12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A8:D12" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Tamaño de la muestra (LINKED_LIST)" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Insertion Sort [ms]" dataDxfId="2"/>
@@ -7529,7 +7097,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7825,21 +7393,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,332 +7421,130 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>5406.25</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>5375</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>5531.25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>29109.375</v>
       </c>
       <c r="C3" s="4">
-        <v>2</v>
+        <v>38968.75</v>
       </c>
       <c r="D3" s="4">
-        <f>D2+15</f>
-        <v>19</v>
+        <v>98921.875</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
       <c r="B4" s="4">
-        <v>30</v>
+        <v>139640.625</v>
       </c>
       <c r="C4" s="4">
-        <f>C3+C2</f>
-        <v>3</v>
+        <v>140953.125</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>140109.375</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>662125</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>661968.75</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <v>662437.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="1">
-        <v>16000</v>
-      </c>
-      <c r="B6" s="4">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A7" s="1">
-        <v>32000</v>
-      </c>
-      <c r="B7" s="4">
-        <v>60</v>
-      </c>
-      <c r="C7" s="4">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" s="1">
-        <v>64000</v>
-      </c>
-      <c r="B8" s="4">
-        <v>70</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="D8" s="4">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A9" s="1">
-        <v>128000</v>
-      </c>
-      <c r="B9" s="4">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" s="1">
-        <v>256000</v>
-      </c>
-      <c r="B10" s="4">
-        <v>90</v>
-      </c>
-      <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="D10" s="4">
-        <f t="shared" si="0"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B11" s="4">
-        <v>100</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A14" s="2" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A15" s="1">
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4">
-        <v>50</v>
+      <c r="B9" s="4">
+        <v>5359.375</v>
       </c>
-      <c r="C15" s="4">
-        <v>2</v>
+      <c r="C9" s="4">
+        <v>5359.375</v>
       </c>
-      <c r="D15" s="4">
-        <v>35</v>
+      <c r="D9" s="4">
+        <v>5531.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A16" s="1">
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4">
-        <v>60</v>
+      <c r="B10" s="4">
+        <v>29578.125</v>
       </c>
-      <c r="C16" s="4">
-        <v>4</v>
+      <c r="C10" s="4">
+        <v>29765.625</v>
       </c>
-      <c r="D16" s="4">
-        <f>D15+43</f>
-        <v>78</v>
+      <c r="D10" s="4">
+        <v>28984.375</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A17" s="1">
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
         <v>4000</v>
       </c>
-      <c r="B17" s="4">
-        <v>70</v>
+      <c r="B11" s="4">
+        <v>140343.375</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" ref="C17:C24" si="2">C16+C15</f>
-        <v>6</v>
+      <c r="C11" s="4">
+        <v>142187.5</v>
       </c>
-      <c r="D17" s="4">
-        <f t="shared" ref="D17:D24" si="3">D16+10</f>
-        <v>88</v>
+      <c r="D11" s="4">
+        <v>141359.375</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A18" s="1">
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
         <v>8000</v>
       </c>
-      <c r="B18" s="4">
-        <v>80</v>
+      <c r="B12" s="4">
+        <v>662022.35</v>
       </c>
-      <c r="C18" s="4">
-        <f t="shared" si="2"/>
-        <v>10</v>
+      <c r="C12" s="4">
+        <v>663198.25</v>
       </c>
-      <c r="D18" s="4">
-        <f t="shared" si="3"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A19" s="1">
-        <v>16000</v>
-      </c>
-      <c r="B19" s="4">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f t="shared" si="3"/>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A20" s="1">
-        <v>32000</v>
-      </c>
-      <c r="B20" s="4">
-        <v>100</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D20" s="4">
-        <f t="shared" si="3"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A21" s="1">
-        <v>64000</v>
-      </c>
-      <c r="B21" s="4">
-        <v>110</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="D21" s="4">
-        <f t="shared" si="3"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A22" s="1">
-        <v>128000</v>
-      </c>
-      <c r="B22" s="4">
-        <v>120</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="2"/>
-        <v>68</v>
-      </c>
-      <c r="D22" s="4">
-        <f t="shared" si="3"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A23" s="1">
-        <v>256000</v>
-      </c>
-      <c r="B23" s="4">
-        <v>130</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="2"/>
-        <v>110</v>
-      </c>
-      <c r="D23" s="4">
-        <f t="shared" si="3"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A24" s="1">
-        <v>512000</v>
-      </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="2"/>
-        <v>178</v>
-      </c>
-      <c r="D24" s="4">
-        <f t="shared" si="3"/>
-        <v>158</v>
+      <c r="D12" s="4">
+        <v>660112.5</v>
       </c>
     </row>
   </sheetData>
@@ -8191,12 +7557,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +7774,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +7811,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>